<commit_message>
actualizacion de produtos en pagina
</commit_message>
<xml_diff>
--- a/src/actualizar_precios/actualizar_precios.xlsx
+++ b/src/actualizar_precios/actualizar_precios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\TeamComunicaciones\automatizadorteam\src\actualizar_precios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\TeamComunicaciones\programa listo\src\actualizar_precios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5135989C-44A2-48B8-A677-787827B65A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9694404B-A4D3-4803-954D-CE0A3E534370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7575" yWindow="1215" windowWidth="14985" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Producto</t>
   </si>
@@ -28,20 +28,31 @@
     <t>Precio</t>
   </si>
   <si>
-    <t>HONOR MAGIC 5 LITE 128GB 6RAM</t>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>producto1</t>
+  </si>
+  <si>
+    <t>producto2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,7 +63,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -60,12 +71,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,36 +397,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1150000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>600000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>